<commit_message>
remove adding pharmacy deposite from list as it has been deprecating and add adminUser in TC006PharmacyDeposit&Return.py
</commit_message>
<xml_diff>
--- a/Library/excelTestCasesSystemTest_SNCH.xlsx
+++ b/Library/excelTestCasesSystemTest_SNCH.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="84">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Pharmacy\TC002ReturnPharmacyInvoice.py</t>
   </si>
   <si>
-    <t>TC017</t>
-  </si>
-  <si>
     <t>TC018</t>
   </si>
   <si>
@@ -109,9 +106,6 @@
   </si>
   <si>
     <t>TC019</t>
-  </si>
-  <si>
-    <t>Pharmacy\TC006PharmacyDeposit&amp;Return.py</t>
   </si>
   <si>
     <t>Pharmacy\TC007CreatePharmacyGoodsReceipt.py</t>
@@ -646,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,19 +669,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -695,7 +689,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
@@ -715,7 +709,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
@@ -735,7 +729,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>4</v>
@@ -752,10 +746,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>4</v>
@@ -772,10 +766,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>4</v>
@@ -792,10 +786,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>4</v>
@@ -812,10 +806,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>4</v>
@@ -832,10 +826,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>4</v>
@@ -852,10 +846,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>4</v>
@@ -872,10 +866,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>4</v>
@@ -895,7 +889,7 @@
         <v>19</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>4</v>
@@ -915,7 +909,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>4</v>
@@ -935,7 +929,7 @@
         <v>23</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>4</v>
@@ -955,7 +949,7 @@
         <v>25</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>4</v>
@@ -972,10 +966,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>4</v>
@@ -992,10 +986,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>4</v>
@@ -1012,10 +1006,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>4</v>
@@ -1024,7 +1018,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -1032,10 +1026,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>4</v>
@@ -1044,7 +1038,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -1052,10 +1046,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>4</v>
@@ -1075,7 +1069,7 @@
         <v>37</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>4</v>
@@ -1084,7 +1078,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -1092,10 +1086,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>4</v>
@@ -1104,7 +1098,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -1115,7 +1109,7 @@
         <v>42</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>4</v>
@@ -1132,10 +1126,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>4</v>
@@ -1152,10 +1146,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>4</v>
@@ -1164,7 +1158,7 @@
         <v>0</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -1172,10 +1166,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>4</v>
@@ -1192,10 +1186,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>4</v>
@@ -1204,7 +1198,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
@@ -1212,10 +1206,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>4</v>
@@ -1224,7 +1218,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -1232,10 +1226,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>4</v>
@@ -1255,7 +1249,7 @@
         <v>55</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>4</v>
@@ -1264,7 +1258,7 @@
         <v>0</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
@@ -1272,10 +1266,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>4</v>
@@ -1284,7 +1278,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
@@ -1295,7 +1289,7 @@
         <v>60</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>4</v>
@@ -1304,7 +1298,7 @@
         <v>0</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
@@ -1312,10 +1306,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>4</v>
@@ -1332,10 +1326,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>4</v>
@@ -1355,7 +1349,7 @@
         <v>72</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>4</v>
@@ -1364,7 +1358,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
@@ -1372,10 +1366,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>4</v>
@@ -1395,7 +1389,7 @@
         <v>75</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>4</v>
@@ -1412,10 +1406,10 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>4</v>
@@ -1424,31 +1418,11 @@
         <v>0</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" s="4">
-        <v>0</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Change in testcase of excelTestCasesSystemTest_SNCH.xlsx
</commit_message>
<xml_diff>
--- a/Library/excelTestCasesSystemTest_SNCH.xlsx
+++ b/Library/excelTestCasesSystemTest_SNCH.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="116">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -114,9 +114,6 @@
     <t>TC021</t>
   </si>
   <si>
-    <t>Pharmacy\Reports\TC002UserCollectionReport.py</t>
-  </si>
-  <si>
     <t>TC023</t>
   </si>
   <si>
@@ -271,13 +268,112 @@
   </si>
   <si>
     <t>Billing\OPbilling\TC009CreateEstimationBill.py</t>
+  </si>
+  <si>
+    <t>Pharmacy\TC004PharmacyStoreManageItem.py</t>
+  </si>
+  <si>
+    <t>Onhold</t>
+  </si>
+  <si>
+    <t>TC015</t>
+  </si>
+  <si>
+    <t>Below Test Actions are currently deprecated</t>
+  </si>
+  <si>
+    <t>Pharmacy\TC006PharmacyDeposit&amp;Return.py</t>
+  </si>
+  <si>
+    <t>Deprecated</t>
+  </si>
+  <si>
+    <t>TC017</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\TC001CashCollectionSummaryReport.py</t>
+  </si>
+  <si>
+    <t>TC020</t>
+  </si>
+  <si>
+    <t>No any such report found</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\TC006Opening&amp;EndingStockSummaryReport.py</t>
+  </si>
+  <si>
+    <t>TC022</t>
+  </si>
+  <si>
+    <t>Reports\TC003SalesDayBookReport.py</t>
+  </si>
+  <si>
+    <t>TC030</t>
+  </si>
+  <si>
+    <t>Reports\TC004PatientCensusReport.py</t>
+  </si>
+  <si>
+    <t>TC031</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Failed due to old Patient</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>EMR-4920</t>
+  </si>
+  <si>
+    <t>Failed due to EMR-4920</t>
+  </si>
+  <si>
+    <t>Script need to maintain</t>
+  </si>
+  <si>
+    <t>Happy Path Testing</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\TC003UserCollectionReport.py</t>
+  </si>
+  <si>
+    <t>EMR-4923</t>
+  </si>
+  <si>
+    <t>Reports\TC007DoctorSummaryReport.py</t>
+  </si>
+  <si>
+    <t>TC034</t>
+  </si>
+  <si>
+    <t>No such report found</t>
+  </si>
+  <si>
+    <t>Reports\TC010DepartmentSummaryReport.py</t>
+  </si>
+  <si>
+    <t>TC037</t>
+  </si>
+  <si>
+    <t>EMR-4926</t>
+  </si>
+  <si>
+    <t>Issues and Requirement changing need to add credit organization in credit billings</t>
+  </si>
+  <si>
+    <t>Requirement changing need to add credit organization in credit billings</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,8 +389,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color theme="1"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -304,6 +414,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -346,7 +480,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -360,6 +494,14 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,13 +782,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="75.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
@@ -655,10 +797,10 @@
     <col min="5" max="5" width="12.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="50.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="17.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -669,27 +811,27 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="H1" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
@@ -700,16 +842,20 @@
       <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="10" t="s">
+        <v>99</v>
+      </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
@@ -724,12 +870,12 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>4</v>
@@ -744,12 +890,12 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>4</v>
@@ -764,12 +910,12 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>4</v>
@@ -784,12 +930,12 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>4</v>
@@ -800,16 +946,22 @@
       <c r="E7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>4</v>
@@ -820,16 +972,22 @@
       <c r="E8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F8" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>4</v>
@@ -840,16 +998,22 @@
       <c r="E9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>4</v>
@@ -864,12 +1028,12 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>4</v>
@@ -884,12 +1048,12 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>4</v>
@@ -904,12 +1068,12 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>4</v>
@@ -924,12 +1088,12 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>4</v>
@@ -940,16 +1104,20 @@
       <c r="E14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="4"/>
+      <c r="F14" s="10" t="s">
+        <v>99</v>
+      </c>
       <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H14" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>4</v>
@@ -964,52 +1132,58 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0</v>
-      </c>
-      <c r="E16" s="5" t="s">
+      <c r="B17" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="4">
-        <v>0</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="4" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>4</v>
@@ -1018,18 +1192,22 @@
         <v>0</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="4"/>
+        <v>89</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>88</v>
+      </c>
       <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>4</v>
@@ -1038,18 +1216,18 @@
         <v>0</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="4" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>4</v>
@@ -1058,18 +1236,18 @@
         <v>0</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="4" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>4</v>
@@ -1078,18 +1256,22 @@
         <v>0</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" s="4"/>
+        <v>91</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="4" t="s">
-        <v>40</v>
+        <v>106</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>4</v>
@@ -1098,18 +1280,18 @@
         <v>0</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="4" t="s">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>4</v>
@@ -1118,18 +1300,22 @@
         <v>0</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F23" s="4"/>
+        <v>94</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H23" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="4" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>4</v>
@@ -1138,18 +1324,18 @@
         <v>0</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="4" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>4</v>
@@ -1158,18 +1344,18 @@
         <v>0</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>4</v>
@@ -1178,18 +1364,18 @@
         <v>0</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="4" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>4</v>
@@ -1198,18 +1384,18 @@
         <v>0</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>4</v>
@@ -1218,18 +1404,18 @@
         <v>0</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="4" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>4</v>
@@ -1238,18 +1424,18 @@
         <v>0</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="4" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>4</v>
@@ -1258,18 +1444,18 @@
         <v>0</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="4" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>4</v>
@@ -1278,18 +1464,22 @@
         <v>0</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F31" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H31" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="4" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>4</v>
@@ -1298,18 +1488,22 @@
         <v>0</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F32" s="4"/>
+        <v>98</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H32" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="4" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>4</v>
@@ -1318,18 +1512,18 @@
         <v>0</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="4" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>4</v>
@@ -1338,18 +1532,22 @@
         <v>0</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>107</v>
+      </c>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="4" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>4</v>
@@ -1358,18 +1556,22 @@
         <v>0</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F35" s="4"/>
+        <v>109</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H35" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="4" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>4</v>
@@ -1378,18 +1580,18 @@
         <v>0</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="4" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>4</v>
@@ -1398,31 +1600,201 @@
         <v>0</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="4">
+        <v>0</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="4">
+        <v>0</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="4">
+        <v>0</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="4">
+        <v>0</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="4">
+        <v>0</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="4">
+        <v>0</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="4">
+        <v>0</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F44" s="4"/>
+      <c r="G44" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="4">
-        <v>0</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
+      <c r="B45" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="4">
+        <v>0</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" s="4">
+        <v>0</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4" t="s">
+        <v>115</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added More TestCase in SNCH in excelTestCasesSystemTest_SNCH.xlsx
</commit_message>
<xml_diff>
--- a/Library/excelTestCasesSystemTest_SNCH.xlsx
+++ b/Library/excelTestCasesSystemTest_SNCH.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="166">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -297,9 +297,6 @@
     <t>No any such report found</t>
   </si>
   <si>
-    <t>Pharmacy\Reports\TC006Opening&amp;EndingStockSummaryReport.py</t>
-  </si>
-  <si>
     <t>TC022</t>
   </si>
   <si>
@@ -367,6 +364,159 @@
   </si>
   <si>
     <t>Pharmacy\Reports\Sales\TC03UserCollectionReport.py</t>
+  </si>
+  <si>
+    <t>Accounting\TC01ClosingFIscalYear.py</t>
+  </si>
+  <si>
+    <t>Accounting\TC03VerifyPosttoAccounting.py</t>
+  </si>
+  <si>
+    <t>ADT\TC010AdmissionDischargeTransferToBePaid.py</t>
+  </si>
+  <si>
+    <t>ADT\TC012DischargeHappyPath.py</t>
+  </si>
+  <si>
+    <t>Billing\OPbilling\TC011CreateCopyOfItemsCashInvoice.py</t>
+  </si>
+  <si>
+    <t>Billing\OPbilling\TC012CreateCopyOfItemsCreditInvoice.py</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\Purchase\TC01ItemWisePurchaseReport.py</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\Purchase\TC02PurchaseSummaryReport.py</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\TC004InvoiceBillingReport.py</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\TC005InvoiceSaleReturnBillingReport.py</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\TC010VerifyPharmacyDashboard.py</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\TC011VerifyStockItemsReport.py</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\Purchase\TC03ReturnToSupplierReport.py</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\Sales\TC01BillWiseSalesReport.py</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\Sales\TC02ItemWiseSalesReport.py</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\Sales\TC008SalesStatement.py</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\Sales\TC009Patient-WiseSalesDetail.py</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\Stock\TC006Opening&amp;EndingStockSummaryReport.py</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\Stock\StockTransferReport.py</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\Stock\TC01SupplierStockReport.py</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\Stock\TC02ExpiryReport.py</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\Stock\TC04NarcoticStockReport.py</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\Stock\TC05ReturnFromCustomerReport.py</t>
+  </si>
+  <si>
+    <t>Radiology\TC001GenerateUSGReport.py</t>
+  </si>
+  <si>
+    <t>Reports\TC001BillingDashboardSummary.py</t>
+  </si>
+  <si>
+    <t>TC046</t>
+  </si>
+  <si>
+    <t>TC047</t>
+  </si>
+  <si>
+    <t>TC048</t>
+  </si>
+  <si>
+    <t>TC049</t>
+  </si>
+  <si>
+    <t>TC050</t>
+  </si>
+  <si>
+    <t>TC051</t>
+  </si>
+  <si>
+    <t>TC052</t>
+  </si>
+  <si>
+    <t>TC053</t>
+  </si>
+  <si>
+    <t>TC054</t>
+  </si>
+  <si>
+    <t>TC055</t>
+  </si>
+  <si>
+    <t>TC056</t>
+  </si>
+  <si>
+    <t>TC057</t>
+  </si>
+  <si>
+    <t>TC058</t>
+  </si>
+  <si>
+    <t>TC059</t>
+  </si>
+  <si>
+    <t>TC060</t>
+  </si>
+  <si>
+    <t>TC061</t>
+  </si>
+  <si>
+    <t>TC062</t>
+  </si>
+  <si>
+    <t>TC063</t>
+  </si>
+  <si>
+    <t>TC064</t>
+  </si>
+  <si>
+    <t>TC065</t>
+  </si>
+  <si>
+    <t>TC066</t>
+  </si>
+  <si>
+    <t>TC067</t>
+  </si>
+  <si>
+    <t>TC068</t>
+  </si>
+  <si>
+    <t>TC069</t>
+  </si>
+  <si>
+    <t>No such report</t>
+  </si>
+  <si>
+    <t>No Such Report</t>
   </si>
 </sst>
 </file>
@@ -442,7 +592,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -465,17 +615,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -493,15 +632,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -782,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -822,7 +961,7 @@
       <c r="G1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="2" t="s">
         <v>77</v>
       </c>
     </row>
@@ -842,12 +981,12 @@
       <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>98</v>
+      <c r="F2" s="8" t="s">
+        <v>97</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -946,14 +1085,14 @@
       <c r="E7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="H7" s="9" t="s">
         <v>101</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -972,14 +1111,14 @@
       <c r="E8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="H8" s="9" t="s">
         <v>101</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -998,19 +1137,19 @@
       <c r="E9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="H9" s="9" t="s">
         <v>101</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="4" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>80</v>
@@ -1030,7 +1169,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="4" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>80</v>
@@ -1045,12 +1184,16 @@
         <v>16</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="G11" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="4" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>80</v>
@@ -1070,7 +1213,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="4" t="s">
-        <v>22</v>
+        <v>119</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>80</v>
@@ -1090,7 +1233,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="4" t="s">
-        <v>23</v>
+        <v>120</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>80</v>
@@ -1104,17 +1247,13 @@
       <c r="E14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="10" t="s">
-        <v>98</v>
-      </c>
+      <c r="F14" s="4"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="4" t="s">
-        <v>103</v>
-      </c>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="4" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>80</v>
@@ -1134,7 +1273,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="4" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>80</v>
@@ -1148,17 +1287,13 @@
       <c r="E16" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F16" s="7" t="s">
-        <v>83</v>
-      </c>
+      <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="8" t="s">
-        <v>85</v>
-      </c>
+      <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="4" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>80</v>
@@ -1174,13 +1309,11 @@
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="4" t="s">
-        <v>104</v>
-      </c>
+      <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="4" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>80</v>
@@ -1194,17 +1327,13 @@
       <c r="E18" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F18" s="9" t="s">
-        <v>87</v>
-      </c>
+      <c r="F18" s="4"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="4" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>80</v>
@@ -1220,11 +1349,13 @@
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
+      <c r="H19" s="4" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="4" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>80</v>
@@ -1244,7 +1375,7 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="4" t="s">
-        <v>89</v>
+        <v>138</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>80</v>
@@ -1258,17 +1389,13 @@
       <c r="E21" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F21" s="7" t="s">
-        <v>83</v>
-      </c>
+      <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="4" t="s">
-        <v>115</v>
+        <v>22</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>80</v>
@@ -1288,31 +1415,31 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="4">
-        <v>0</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>83</v>
+      <c r="F23" s="8" t="s">
+        <v>97</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="4" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>80</v>
@@ -1332,7 +1459,7 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="4" t="s">
-        <v>114</v>
+        <v>82</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>80</v>
@@ -1346,13 +1473,17 @@
       <c r="E25" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="4"/>
+      <c r="F25" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
+      <c r="H25" s="11" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="4" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>80</v>
@@ -1368,11 +1499,13 @@
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
+      <c r="H26" s="4" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="4" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>80</v>
@@ -1386,13 +1519,17 @@
       <c r="E27" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F27" s="4"/>
+      <c r="F27" s="7" t="s">
+        <v>87</v>
+      </c>
       <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
+      <c r="H27" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="4" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>80</v>
@@ -1412,7 +1549,7 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>80</v>
@@ -1432,7 +1569,7 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="4" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>80</v>
@@ -1446,61 +1583,57 @@
       <c r="E30" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F30" s="4"/>
+      <c r="F30" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
+      <c r="H30" s="4" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="4">
+        <v>0</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="4">
-        <v>0</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>83</v>
-      </c>
+      <c r="F31" s="4"/>
       <c r="G31" s="4"/>
-      <c r="H31" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="H31" s="4"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="4">
-        <v>0</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>83</v>
-      </c>
+      <c r="F32" s="4"/>
       <c r="G32" s="4"/>
-      <c r="H32" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="H32" s="4"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>80</v>
@@ -1520,7 +1653,7 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="4" t="s">
-        <v>48</v>
+        <v>125</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>80</v>
@@ -1534,41 +1667,33 @@
       <c r="E34" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F34" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="G34" s="12" t="s">
-        <v>105</v>
-      </c>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
       <c r="H34" s="4"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="4">
+        <v>0</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" s="4">
-        <v>0</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>83</v>
-      </c>
+      <c r="F35" s="4"/>
       <c r="G35" s="4"/>
-      <c r="H35" s="4" t="s">
-        <v>108</v>
-      </c>
+      <c r="H35" s="4"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="4" t="s">
-        <v>51</v>
+        <v>121</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>80</v>
@@ -1588,7 +1713,7 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="4" t="s">
-        <v>53</v>
+        <v>122</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>80</v>
@@ -1608,31 +1733,27 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="4">
+        <v>0</v>
+      </c>
+      <c r="E38" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="4">
-        <v>0</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>83</v>
-      </c>
+      <c r="F38" s="4"/>
       <c r="G38" s="4"/>
-      <c r="H38" s="4" t="s">
-        <v>108</v>
-      </c>
+      <c r="H38" s="4"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="4" t="s">
-        <v>56</v>
+        <v>114</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>80</v>
@@ -1651,8 +1772,8 @@
       <c r="H39" s="4"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="4" t="s">
-        <v>58</v>
+      <c r="A40" s="12" t="s">
+        <v>128</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>80</v>
@@ -1666,13 +1787,17 @@
       <c r="E40" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F40" s="4"/>
+      <c r="F40" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
+      <c r="H40" s="4" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="4" t="s">
-        <v>69</v>
+      <c r="A41" s="12" t="s">
+        <v>129</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>80</v>
@@ -1692,7 +1817,7 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="4" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>80</v>
@@ -1712,7 +1837,7 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="4" t="s">
-        <v>70</v>
+        <v>130</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>80</v>
@@ -1732,7 +1857,7 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="4" t="s">
-        <v>71</v>
+        <v>131</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>80</v>
@@ -1747,16 +1872,12 @@
         <v>57</v>
       </c>
       <c r="F44" s="4"/>
-      <c r="G44" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="H44" s="4" t="s">
-        <v>112</v>
-      </c>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="4" t="s">
-        <v>73</v>
+        <v>133</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>80</v>
@@ -1776,7 +1897,7 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="4" t="s">
-        <v>72</v>
+        <v>134</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>80</v>
@@ -1792,9 +1913,515 @@
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
-      <c r="H46" s="4" t="s">
-        <v>113</v>
-      </c>
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="4">
+        <v>0</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" s="4">
+        <v>0</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="4">
+        <v>0</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="4">
+        <v>0</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="4">
+        <v>0</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="4">
+        <v>0</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" s="4">
+        <v>0</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" s="4">
+        <v>0</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" s="4">
+        <v>0</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56" s="4">
+        <v>0</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="4">
+        <v>0</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" s="4">
+        <v>0</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" s="4">
+        <v>0</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" s="4">
+        <v>0</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" s="4">
+        <v>0</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" s="4">
+        <v>0</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F62" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G62" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="H62" s="4"/>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D63" s="4">
+        <v>0</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64" s="4">
+        <v>0</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" s="4">
+        <v>0</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D66" s="4">
+        <v>0</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G66" s="4"/>
+      <c r="H66" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D67" s="4">
+        <v>0</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D68" s="4">
+        <v>0</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D69" s="4">
+        <v>0</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F69" s="4"/>
+      <c r="G69" s="4"/>
+      <c r="H69" s="4"/>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D70" s="4">
+        <v>0</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F70" s="4"/>
+      <c r="G70" s="4"/>
+      <c r="H70" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changes in remarks and add bugid in excelTestCasesSystemTest_SNCH.xlsx
</commit_message>
<xml_diff>
--- a/Library/excelTestCasesSystemTest_SNCH.xlsx
+++ b/Library/excelTestCasesSystemTest_SNCH.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="168">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -517,6 +517,12 @@
   </si>
   <si>
     <t>No Such Report</t>
+  </si>
+  <si>
+    <t>EMR-4700</t>
+  </si>
+  <si>
+    <t>Enhancement on billing Dashboard</t>
   </si>
 </sst>
 </file>
@@ -923,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2136,8 +2142,12 @@
         <v>150</v>
       </c>
       <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
+      <c r="G57" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="4" t="s">

</xml_diff>

<commit_message>
change in TestCases in excelTestCasesSystemTest_SNCH.xlsx as refer to excelResultSystemTest_SNCHVV2.1.9AA_Hotfix1
</commit_message>
<xml_diff>
--- a/Library/excelTestCasesSystemTest_SNCH.xlsx
+++ b/Library/excelTestCasesSystemTest_SNCH.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="133">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -195,9 +195,6 @@
     <t>TC043</t>
   </si>
   <si>
-    <t>Reports\TC012TotalAdmittedPatientsReport.py</t>
-  </si>
-  <si>
     <t>TC044</t>
   </si>
   <si>
@@ -267,54 +264,24 @@
     <t>Billing\OPbilling\TC009CreateEstimationBill.py</t>
   </si>
   <si>
-    <t>Pharmacy\TC004PharmacyStoreManageItem.py</t>
-  </si>
-  <si>
-    <t>Onhold</t>
-  </si>
-  <si>
     <t>TC015</t>
   </si>
   <si>
-    <t>Below Test Actions are currently deprecated</t>
-  </si>
-  <si>
-    <t>Pharmacy\TC006PharmacyDeposit&amp;Return.py</t>
-  </si>
-  <si>
-    <t>Deprecated</t>
-  </si>
-  <si>
     <t>TC017</t>
   </si>
   <si>
-    <t>Pharmacy\Reports\TC001CashCollectionSummaryReport.py</t>
-  </si>
-  <si>
     <t>TC020</t>
   </si>
   <si>
-    <t>No any such report found</t>
-  </si>
-  <si>
     <t>TC022</t>
   </si>
   <si>
-    <t>Reports\TC003SalesDayBookReport.py</t>
-  </si>
-  <si>
     <t>TC030</t>
   </si>
   <si>
-    <t>Reports\TC004PatientCensusReport.py</t>
-  </si>
-  <si>
     <t>TC031</t>
   </si>
   <si>
-    <t>Passed</t>
-  </si>
-  <si>
     <t>Failed due to old Patient</t>
   </si>
   <si>
@@ -336,18 +303,9 @@
     <t>EMR-4923</t>
   </si>
   <si>
-    <t>Reports\TC007DoctorSummaryReport.py</t>
-  </si>
-  <si>
     <t>TC034</t>
   </si>
   <si>
-    <t>No such report found</t>
-  </si>
-  <si>
-    <t>Reports\TC010DepartmentSummaryReport.py</t>
-  </si>
-  <si>
     <t>TC037</t>
   </si>
   <si>
@@ -366,24 +324,12 @@
     <t>Pharmacy\Reports\Sales\TC03UserCollectionReport.py</t>
   </si>
   <si>
-    <t>Accounting\TC01ClosingFIscalYear.py</t>
-  </si>
-  <si>
-    <t>Accounting\TC03VerifyPosttoAccounting.py</t>
-  </si>
-  <si>
     <t>ADT\TC010AdmissionDischargeTransferToBePaid.py</t>
   </si>
   <si>
     <t>ADT\TC012DischargeHappyPath.py</t>
   </si>
   <si>
-    <t>Billing\OPbilling\TC011CreateCopyOfItemsCashInvoice.py</t>
-  </si>
-  <si>
-    <t>Billing\OPbilling\TC012CreateCopyOfItemsCreditInvoice.py</t>
-  </si>
-  <si>
     <t>Pharmacy\Reports\Purchase\TC01ItemWisePurchaseReport.py</t>
   </si>
   <si>
@@ -405,9 +351,6 @@
     <t>Pharmacy\Reports\Purchase\TC03ReturnToSupplierReport.py</t>
   </si>
   <si>
-    <t>Pharmacy\Reports\Sales\TC01BillWiseSalesReport.py</t>
-  </si>
-  <si>
     <t>Pharmacy\Reports\Sales\TC02ItemWiseSalesReport.py</t>
   </si>
   <si>
@@ -417,9 +360,6 @@
     <t>Pharmacy\Reports\Sales\TC009Patient-WiseSalesDetail.py</t>
   </si>
   <si>
-    <t>Pharmacy\Reports\Stock\TC006Opening&amp;EndingStockSummaryReport.py</t>
-  </si>
-  <si>
     <t>Pharmacy\Reports\Stock\StockTransferReport.py</t>
   </si>
   <si>
@@ -471,65 +411,20 @@
     <t>TC055</t>
   </si>
   <si>
-    <t>TC056</t>
-  </si>
-  <si>
-    <t>TC057</t>
-  </si>
-  <si>
-    <t>TC058</t>
-  </si>
-  <si>
-    <t>TC059</t>
-  </si>
-  <si>
-    <t>TC060</t>
-  </si>
-  <si>
-    <t>TC061</t>
-  </si>
-  <si>
-    <t>TC062</t>
-  </si>
-  <si>
-    <t>TC063</t>
-  </si>
-  <si>
-    <t>TC064</t>
-  </si>
-  <si>
-    <t>TC065</t>
-  </si>
-  <si>
-    <t>TC066</t>
-  </si>
-  <si>
-    <t>TC067</t>
-  </si>
-  <si>
-    <t>TC068</t>
-  </si>
-  <si>
-    <t>TC069</t>
-  </si>
-  <si>
-    <t>No such report</t>
-  </si>
-  <si>
-    <t>No Such Report</t>
-  </si>
-  <si>
     <t>EMR-4700</t>
   </si>
   <si>
     <t>Enhancement on billing Dashboard</t>
+  </si>
+  <si>
+    <t>Need Scripting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -546,12 +441,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9.8000000000000007"/>
-      <color theme="1"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
@@ -560,7 +449,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -570,24 +459,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -625,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -639,13 +510,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -927,13 +792,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H70"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G21" sqref="F21:G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="75.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
@@ -945,7 +810,7 @@
     <col min="8" max="8" width="50.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17.25" customHeight="1">
+    <row r="1" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -956,27 +821,27 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
@@ -987,20 +852,18 @@
       <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>97</v>
-      </c>
+      <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
@@ -1015,12 +878,12 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>4</v>
@@ -1035,12 +898,12 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>4</v>
@@ -1055,12 +918,12 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>4</v>
@@ -1075,12 +938,12 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>4</v>
@@ -1091,22 +954,22 @@
       <c r="E7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="F7" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>4</v>
@@ -1117,22 +980,22 @@
       <c r="E8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="F8" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>4</v>
@@ -1143,22 +1006,22 @@
       <c r="E9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="F9" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>4</v>
@@ -1173,12 +1036,12 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>4</v>
@@ -1190,19 +1053,19 @@
         <v>16</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="10" t="s">
-        <v>110</v>
+      <c r="G11" s="7" t="s">
+        <v>96</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>4</v>
@@ -1217,12 +1080,12 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>119</v>
+        <v>78</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>4</v>
@@ -1237,12 +1100,12 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>120</v>
+        <v>68</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>4</v>
@@ -1257,12 +1120,12 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>4</v>
@@ -1277,12 +1140,12 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>4</v>
@@ -1291,18 +1154,18 @@
         <v>0</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>4</v>
@@ -1315,14 +1178,16 @@
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="H17" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>4</v>
@@ -1331,18 +1196,18 @@
         <v>0</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>72</v>
+        <v>118</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>4</v>
@@ -1355,16 +1220,14 @@
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
-      <c r="H19" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>4</v>
@@ -1379,12 +1242,12 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>138</v>
+        <v>23</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>4</v>
@@ -1393,18 +1256,20 @@
         <v>0</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="H21" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>4</v>
@@ -1419,12 +1284,12 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>4</v>
@@ -1433,22 +1298,20 @@
         <v>0</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>97</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>4</v>
@@ -1463,12 +1326,12 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>4</v>
@@ -1479,20 +1342,16 @@
       <c r="E25" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="6" t="s">
-        <v>83</v>
-      </c>
+      <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>27</v>
+        <v>105</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>4</v>
@@ -1505,16 +1364,14 @@
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
-      <c r="H26" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>4</v>
@@ -1525,20 +1382,16 @@
       <c r="E27" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F27" s="7" t="s">
-        <v>87</v>
-      </c>
+      <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-      <c r="H27" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>4</v>
@@ -1553,12 +1406,12 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>4</v>
@@ -1573,12 +1426,12 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>4</v>
@@ -1589,20 +1442,16 @@
       <c r="E30" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F30" s="6" t="s">
-        <v>83</v>
-      </c>
+      <c r="F30" s="4"/>
       <c r="G30" s="4"/>
-      <c r="H30" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>4</v>
@@ -1611,18 +1460,18 @@
         <v>0</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>4</v>
@@ -1631,18 +1480,18 @@
         <v>0</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>34</v>
+        <v>109</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>4</v>
@@ -1657,12 +1506,12 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>4</v>
@@ -1677,12 +1526,12 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="4" t="s">
-        <v>126</v>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>110</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>4</v>
@@ -1691,18 +1540,18 @@
         <v>0</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>4</v>
@@ -1717,12 +1566,12 @@
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>4</v>
@@ -1735,14 +1584,16 @@
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="H37" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>4</v>
@@ -1751,18 +1602,18 @@
         <v>0</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>4</v>
@@ -1777,12 +1628,12 @@
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
     </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="12" t="s">
-        <v>128</v>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>114</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>4</v>
@@ -1793,20 +1644,16 @@
       <c r="E40" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F40" s="6" t="s">
-        <v>83</v>
-      </c>
+      <c r="F40" s="4"/>
       <c r="G40" s="4"/>
-      <c r="H40" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="12" t="s">
-        <v>129</v>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>4</v>
@@ -1821,12 +1668,12 @@
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>4</v>
@@ -1841,12 +1688,12 @@
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>4</v>
@@ -1861,12 +1708,12 @@
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>131</v>
+        <v>38</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>4</v>
@@ -1881,12 +1728,12 @@
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>133</v>
+        <v>40</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>4</v>
@@ -1895,18 +1742,18 @@
         <v>0</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>134</v>
+        <v>101</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>4</v>
@@ -1915,18 +1762,18 @@
         <v>0</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>135</v>
+        <v>102</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>4</v>
@@ -1935,18 +1782,18 @@
         <v>0</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>136</v>
+        <v>41</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>4</v>
@@ -1955,18 +1802,18 @@
         <v>0</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>137</v>
+        <v>77</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>4</v>
@@ -1975,18 +1822,18 @@
         <v>0</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>4</v>
@@ -1995,22 +1842,22 @@
         <v>0</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G50" s="4"/>
+        <v>123</v>
+      </c>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H50" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>4</v>
@@ -2019,18 +1866,18 @@
         <v>0</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>4</v>
@@ -2039,18 +1886,18 @@
         <v>0</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>117</v>
+        <v>48</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>4</v>
@@ -2059,18 +1906,22 @@
         <v>0</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="F53" s="4"/>
-      <c r="G53" s="4"/>
+        <v>126</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>93</v>
+      </c>
       <c r="H53" s="4"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>4</v>
@@ -2079,18 +1930,18 @@
         <v>0</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>4</v>
@@ -2099,18 +1950,18 @@
         <v>0</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>4</v>
@@ -2119,319 +1970,11 @@
         <v>0</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D57" s="4">
-        <v>0</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="H57" s="4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D58" s="4">
-        <v>0</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
-      <c r="H58" s="4"/>
-    </row>
-    <row r="59" spans="1:8">
-      <c r="A59" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D59" s="4">
-        <v>0</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="F59" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G59" s="4"/>
-      <c r="H59" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
-      <c r="A60" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D60" s="4">
-        <v>0</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G60" s="4"/>
-      <c r="H60" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
-      <c r="A61" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D61" s="4">
-        <v>0</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F61" s="4"/>
-      <c r="G61" s="4"/>
-      <c r="H61" s="4"/>
-    </row>
-    <row r="62" spans="1:8">
-      <c r="A62" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D62" s="4">
-        <v>0</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F62" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G62" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="H62" s="4"/>
-    </row>
-    <row r="63" spans="1:8">
-      <c r="A63" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D63" s="4">
-        <v>0</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F63" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8">
-      <c r="A64" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D64" s="4">
-        <v>0</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="4"/>
-    </row>
-    <row r="65" spans="1:8">
-      <c r="A65" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D65" s="4">
-        <v>0</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F65" s="4"/>
-      <c r="G65" s="4"/>
-      <c r="H65" s="4"/>
-    </row>
-    <row r="66" spans="1:8">
-      <c r="A66" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D66" s="4">
-        <v>0</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="F66" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G66" s="4"/>
-      <c r="H66" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
-      <c r="A67" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D67" s="4">
-        <v>0</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="F67" s="4"/>
-      <c r="G67" s="4"/>
-      <c r="H67" s="4"/>
-    </row>
-    <row r="68" spans="1:8">
-      <c r="A68" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D68" s="4">
-        <v>0</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="F68" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G68" s="4"/>
-      <c r="H68" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
-      <c r="A69" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D69" s="4">
-        <v>0</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="F69" s="4"/>
-      <c r="G69" s="4"/>
-      <c r="H69" s="4"/>
-    </row>
-    <row r="70" spans="1:8">
-      <c r="A70" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D70" s="4">
-        <v>0</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="F70" s="4"/>
-      <c r="G70" s="4"/>
-      <c r="H70" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>